<commit_message>
The generation of the document "Notification of the arrival of a foreign worker" and the document "Payment order for payment of an advance payment"
</commit_message>
<xml_diff>
--- a/document_generation/document_generation_app/document_templates/about_arrival.xlsx
+++ b/document_generation/document_generation_app/document_templates/about_arrival.xlsx
@@ -8,28 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Document_generation_service\document_generation\document_generation_app\document_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFDD7EB-3052-4C28-832E-30BDF5E237E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF19F5F-9CBB-4CD8-9844-8EC5A5A9D368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="стр.1" sheetId="1" r:id="rId1"/>
-    <sheet name="стр.2" sheetId="2" r:id="rId2"/>
-    <sheet name="стр.3" sheetId="3" r:id="rId3"/>
-    <sheet name="стр.4" sheetId="4" r:id="rId4"/>
+    <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet 2" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet 3" sheetId="3" r:id="rId3"/>
+    <sheet name="sheet 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">стр.1!$A$1:$DQ$60</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">стр.2!$A$1:$DQ$63</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">стр.3!$A$1:$DQ$69</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">стр.4!$A$1:$DQ$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'sheet 1'!$A$1:$DQ$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'sheet 2'!$A$1:$DQ$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'sheet 3'!$A$1:$DQ$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'sheet 4'!$A$1:$DQ$57</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
   <si>
     <t>Приложение № 4</t>
   </si>
@@ -1401,21 +1401,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DQ60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="BO44" sqref="BO44:BQ44"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="BJ52" sqref="BJ52:CJ52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="0.7109375" style="6"/>
-    <col min="8" max="8" width="0.7109375" style="6" customWidth="1"/>
-    <col min="9" max="35" width="0.7109375" style="6"/>
-    <col min="36" max="36" width="0.7109375" style="6" customWidth="1"/>
-    <col min="37" max="71" width="0.7109375" style="6"/>
-    <col min="72" max="72" width="0.7109375" style="6" customWidth="1"/>
-    <col min="73" max="107" width="0.7109375" style="6"/>
-    <col min="108" max="108" width="0.7109375" style="6" customWidth="1"/>
-    <col min="109" max="16384" width="0.7109375" style="6"/>
+    <col min="1" max="16384" width="0.7109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:121" s="43" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4826,7 +4818,9 @@
       <c r="BX44" s="77"/>
       <c r="BY44" s="77"/>
       <c r="BZ44" s="64"/>
-      <c r="CA44" s="61"/>
+      <c r="CA44" s="61" t="s">
+        <v>105</v>
+      </c>
       <c r="CB44" s="62"/>
       <c r="CC44" s="63"/>
       <c r="CD44" s="59" t="s">
@@ -20842,8 +20836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DQ57"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31:AB31"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z30:BQ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>